<commit_message>
conceptversie 0807 naar Teams
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/xlsxUIT/OPEN/AK_OPEN.xlsx
+++ b/public/cohort/fileExcel/xlsxUIT/OPEN/AK_OPEN.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
   <si>
     <t>betekenis kleuren</t>
   </si>
@@ -972,6 +972,9 @@
     <t>PW Systeem Aarde</t>
   </si>
   <si>
+    <t>kies...</t>
+  </si>
+  <si>
     <t>Katern Systeem Aarde</t>
   </si>
   <si>
@@ -984,7 +987,14 @@
     <t>E1</t>
   </si>
   <si>
-    <t>Katern BraziliÃ«</t>
+    <t xml:space="preserve">Katern Brazilië aangevuld met CE stof: Systeem Aarde &amp; Arm en Rijk Hoofdstuk 3 en 4 exclusief CE stof Wonen in Nederland
+</t>
+  </si>
+  <si>
+    <t>D1, D2, C2, C3, B1, B2</t>
+  </si>
+  <si>
+    <t>Katern Brazilië</t>
   </si>
   <si>
     <t>D1, D2</t>
@@ -1003,6 +1013,9 @@
   </si>
   <si>
     <t>Onderzoek m.b.t. een sociaal of fysisch geografisch onderwerp, gericht op de eigen omgeving</t>
+  </si>
+  <si>
+    <t>A1, A2, E2</t>
   </si>
   <si>
     <t>Proefwerk Arm en Rijk</t>
@@ -2096,7 +2109,7 @@
       </c>
       <c r="F2" s="43">
         <f>SUM(AF6:AF35)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="49" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
@@ -2242,7 +2255,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2596,7 +2609,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2968,7 +2981,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I18" s="45">
         <v>1</v>
@@ -2983,7 +2996,7 @@
       </c>
       <c r="N18" s="46"/>
       <c r="O18" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P18" s="32"/>
       <c r="R18" s="7">
@@ -3028,7 +3041,7 @@
       </c>
       <c r="AB18" s="7">
         <f>IF(AND(OR($O18=instellingen!$I$3,$O18=instellingen!$I$4),OR($M18=instellingen!$I$2,$M18=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="7">
         <f>IF(AND($O18=instellingen!$I$2,$M18=instellingen!$I$3),1,0)</f>
@@ -3044,7 +3057,7 @@
       </c>
       <c r="AF18" s="8">
         <f>SUM(R18:AE18)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:32" customHeight="1" ht="72">
@@ -3073,7 +3086,7 @@
       </c>
       <c r="N19" s="46"/>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P19" s="32"/>
       <c r="R19" s="7">
@@ -3118,7 +3131,7 @@
       </c>
       <c r="AB19" s="7">
         <f>IF(AND(OR($O19=instellingen!$I$3,$O19=instellingen!$I$4),OR($M19=instellingen!$I$2,$M19=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="7">
         <f>IF(AND($O19=instellingen!$I$2,$M19=instellingen!$I$3),1,0)</f>
@@ -3134,7 +3147,7 @@
       </c>
       <c r="AF19" s="8">
         <f>SUM(R19:AE19)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1" ht="72">
@@ -3146,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I20" s="45">
         <v>3</v>
@@ -3165,10 +3178,10 @@
         <v>3</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="R20" s="7">
         <f>IF(OR(AND($G20&lt;&gt;instellingen!$G$2,ISBLANK($H20)),AND($G20=instellingen!$G$2,$H20&lt;&gt;"")),1,0)</f>
@@ -3240,7 +3253,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="I21" s="45">
         <v>3</v>
@@ -3259,10 +3272,10 @@
         <v>1</v>
       </c>
       <c r="O21" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P21" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="R21" s="7">
         <f>IF(OR(AND($G21&lt;&gt;instellingen!$G$2,ISBLANK($H21)),AND($G21=instellingen!$G$2,$H21&lt;&gt;"")),1,0)</f>
@@ -3334,7 +3347,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I22" s="45">
         <v>3</v>
@@ -3354,7 +3367,7 @@
         <v>11</v>
       </c>
       <c r="P22" s="32" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="R22" s="7">
         <f>IF(OR(AND($G22&lt;&gt;instellingen!$G$2,ISBLANK($H22)),AND($G22=instellingen!$G$2,$H22&lt;&gt;"")),1,0)</f>
@@ -3426,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I23" s="45">
         <v>3</v>
@@ -3445,10 +3458,10 @@
         <v>2</v>
       </c>
       <c r="O23" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P23" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R23" s="7">
         <f>IF(OR(AND($G23&lt;&gt;instellingen!$G$2,ISBLANK($H23)),AND($G23=instellingen!$G$2,$H23&lt;&gt;"")),1,0)</f>
@@ -3683,7 +3696,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I30" s="45"/>
       <c r="J30" s="29" t="s">
@@ -3700,10 +3713,10 @@
         <v>3</v>
       </c>
       <c r="O30" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P30" s="32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="R30" s="7">
         <f>IF(OR(AND($G30&lt;&gt;instellingen!$G$2,ISBLANK($H30)),AND($G30=instellingen!$G$2,$H30&lt;&gt;"")),1,0)</f>
@@ -3775,7 +3788,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I31" s="45"/>
       <c r="J31" s="29" t="s">
@@ -3792,10 +3805,10 @@
         <v>4</v>
       </c>
       <c r="O31" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P31" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="R31" s="7">
         <f>IF(OR(AND($G31&lt;&gt;instellingen!$G$2,ISBLANK($H31)),AND($G31=instellingen!$G$2,$H31&lt;&gt;"")),1,0)</f>
@@ -3867,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I32" s="45"/>
       <c r="J32" s="29" t="s">
@@ -3884,10 +3897,10 @@
         <v>4</v>
       </c>
       <c r="O32" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="R32" s="7">
         <f>IF(OR(AND($G32&lt;&gt;instellingen!$G$2,ISBLANK($H32)),AND($G32=instellingen!$G$2,$H32&lt;&gt;"")),1,0)</f>
@@ -4570,7 +4583,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -4924,7 +4937,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5951,7 +5964,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I30" s="45"/>
       <c r="J30" s="29" t="s">
@@ -5968,10 +5981,10 @@
         <v>3</v>
       </c>
       <c r="O30" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P30" s="32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="R30" s="7">
         <f>IF(OR(AND($G30&lt;&gt;instellingen!$G$2,ISBLANK($H30)),AND($G30=instellingen!$G$2,$H30&lt;&gt;"")),1,0)</f>
@@ -6043,7 +6056,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I31" s="45"/>
       <c r="J31" s="29" t="s">
@@ -6060,10 +6073,10 @@
         <v>4</v>
       </c>
       <c r="O31" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P31" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="R31" s="7">
         <f>IF(OR(AND($G31&lt;&gt;instellingen!$G$2,ISBLANK($H31)),AND($G31=instellingen!$G$2,$H31&lt;&gt;"")),1,0)</f>
@@ -6135,7 +6148,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I32" s="45"/>
       <c r="J32" s="29" t="s">
@@ -6152,10 +6165,10 @@
         <v>4</v>
       </c>
       <c r="O32" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="R32" s="7">
         <f>IF(OR(AND($G32&lt;&gt;instellingen!$G$2,ISBLANK($H32)),AND($G32=instellingen!$G$2,$H32&lt;&gt;"")),1,0)</f>
@@ -7367,7 +7380,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633402778</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7846,7 +7859,7 @@
         <v>5</v>
       </c>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P19" s="32" t="s">
         <v>75</v>
@@ -7938,7 +7951,7 @@
         <v>5</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
         <v>77</v>
@@ -8030,7 +8043,7 @@
         <v>5</v>
       </c>
       <c r="O21" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P21" s="32" t="s">
         <v>79</v>
@@ -9649,7 +9662,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633402778</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -10128,7 +10141,7 @@
         <v>5</v>
       </c>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P19" s="32" t="s">
         <v>75</v>
@@ -10220,7 +10233,7 @@
         <v>5</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
         <v>77</v>
@@ -10312,7 +10325,7 @@
         <v>5</v>
       </c>
       <c r="O21" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P21" s="32" t="s">
         <v>79</v>
@@ -11431,7 +11444,7 @@
       </c>
       <c r="F2" s="43">
         <f>SUM(AF6:AF35)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" s="49" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
@@ -11604,7 +11617,7 @@
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P6" s="32"/>
       <c r="R6" s="7">
@@ -11649,7 +11662,7 @@
       </c>
       <c r="AB6" s="7">
         <f>IF(AND(OR($O6=instellingen!$I$3,$O6=instellingen!$I$4),OR($M6=instellingen!$I$2,$M6=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="7">
         <f>IF(AND($O6=instellingen!$I$2,$M6=instellingen!$I$3),1,0)</f>
@@ -11665,7 +11678,7 @@
       </c>
       <c r="AF6" s="8">
         <f>SUM(R6:AE6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1" ht="72">
@@ -11702,7 +11715,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P7" s="32" t="s">
         <v>84</v>
@@ -11797,7 +11810,7 @@
         <v>8</v>
       </c>
       <c r="N8" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" s="31" t="s">
         <v>11</v>
@@ -11899,7 +11912,7 @@
       </c>
       <c r="N9" s="46"/>
       <c r="O9" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P9" s="32"/>
       <c r="R9" s="7">
@@ -11944,7 +11957,7 @@
       </c>
       <c r="AB9" s="7">
         <f>IF(AND(OR($O9=instellingen!$I$3,$O9=instellingen!$I$4),OR($M9=instellingen!$I$2,$M9=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="7">
         <f>IF(AND($O9=instellingen!$I$2,$M9=instellingen!$I$3),1,0)</f>
@@ -11960,7 +11973,7 @@
       </c>
       <c r="AF9" s="8">
         <f>SUM(R9:AE9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:32" customHeight="1" ht="72">
@@ -11969,7 +11982,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633402778</v>
       </c>
       <c r="D10" s="2">
         <v>996</v>
@@ -11998,7 +12011,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P10" s="32" t="s">
         <v>89</v>
@@ -12097,7 +12110,7 @@
       </c>
       <c r="N11" s="46"/>
       <c r="O11" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P11" s="32"/>
       <c r="R11" s="7">
@@ -12142,7 +12155,7 @@
       </c>
       <c r="AB11" s="7">
         <f>IF(AND(OR($O11=instellingen!$I$3,$O11=instellingen!$I$4),OR($M11=instellingen!$I$2,$M11=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="7">
         <f>IF(AND($O11=instellingen!$I$2,$M11=instellingen!$I$3),1,0)</f>
@@ -12158,7 +12171,7 @@
       </c>
       <c r="AF11" s="8">
         <f>SUM(R11:AE11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -13725,7 +13738,7 @@
       </c>
       <c r="F2" s="43">
         <f>SUM(AF6:AF35)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" s="49" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
@@ -13898,7 +13911,7 @@
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P6" s="32"/>
       <c r="R6" s="7">
@@ -13943,7 +13956,7 @@
       </c>
       <c r="AB6" s="7">
         <f>IF(AND(OR($O6=instellingen!$I$3,$O6=instellingen!$I$4),OR($M6=instellingen!$I$2,$M6=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="7">
         <f>IF(AND($O6=instellingen!$I$2,$M6=instellingen!$I$3),1,0)</f>
@@ -13959,7 +13972,7 @@
       </c>
       <c r="AF6" s="8">
         <f>SUM(R6:AE6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1" ht="72">
@@ -13996,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="O7" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P7" s="32" t="s">
         <v>84</v>
@@ -14193,7 +14206,7 @@
       </c>
       <c r="N9" s="46"/>
       <c r="O9" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P9" s="32"/>
       <c r="R9" s="7">
@@ -14238,7 +14251,7 @@
       </c>
       <c r="AB9" s="7">
         <f>IF(AND(OR($O9=instellingen!$I$3,$O9=instellingen!$I$4),OR($M9=instellingen!$I$2,$M9=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="7">
         <f>IF(AND($O9=instellingen!$I$2,$M9=instellingen!$I$3),1,0)</f>
@@ -14254,7 +14267,7 @@
       </c>
       <c r="AF9" s="8">
         <f>SUM(R9:AE9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:32" customHeight="1" ht="72">
@@ -14263,7 +14276,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2">
         <v>175</v>
@@ -14292,7 +14305,7 @@
         <v>1</v>
       </c>
       <c r="O10" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P10" s="32" t="s">
         <v>89</v>
@@ -14391,7 +14404,7 @@
       </c>
       <c r="N11" s="46"/>
       <c r="O11" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P11" s="32"/>
       <c r="R11" s="7">
@@ -14436,7 +14449,7 @@
       </c>
       <c r="AB11" s="7">
         <f>IF(AND(OR($O11=instellingen!$I$3,$O11=instellingen!$I$4),OR($M11=instellingen!$I$2,$M11=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="7">
         <f>IF(AND($O11=instellingen!$I$2,$M11=instellingen!$I$3),1,0)</f>
@@ -14452,7 +14465,7 @@
       </c>
       <c r="AF11" s="8">
         <f>SUM(R11:AE11)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -14655,7 +14668,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I18" s="45"/>
       <c r="J18" s="29" t="s">
@@ -14672,10 +14685,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P18" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R18" s="7">
         <f>IF(OR(AND($G18&lt;&gt;instellingen!$G$2,ISBLANK($H18)),AND($G18=instellingen!$G$2,$H18&lt;&gt;"")),1,0)</f>
@@ -14747,7 +14760,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" s="45"/>
       <c r="J19" s="29" t="s">
@@ -14764,10 +14777,10 @@
         <v>2</v>
       </c>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P19" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R19" s="7">
         <f>IF(OR(AND($G19&lt;&gt;instellingen!$G$2,ISBLANK($H19)),AND($G19=instellingen!$G$2,$H19&lt;&gt;"")),1,0)</f>
@@ -14839,7 +14852,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I20" s="45"/>
       <c r="J20" s="29" t="s">
@@ -14856,10 +14869,10 @@
         <v>2</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R20" s="7">
         <f>IF(OR(AND($G20&lt;&gt;instellingen!$G$2,ISBLANK($H20)),AND($G20=instellingen!$G$2,$H20&lt;&gt;"")),1,0)</f>
@@ -16549,7 +16562,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -16921,7 +16934,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I18" s="45"/>
       <c r="J18" s="29" t="s">
@@ -16938,10 +16951,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P18" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R18" s="7">
         <f>IF(OR(AND($G18&lt;&gt;instellingen!$G$2,ISBLANK($H18)),AND($G18=instellingen!$G$2,$H18&lt;&gt;"")),1,0)</f>
@@ -17013,7 +17026,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" s="45"/>
       <c r="J19" s="29" t="s">
@@ -17030,10 +17043,10 @@
         <v>2</v>
       </c>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P19" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R19" s="7">
         <f>IF(OR(AND($G19&lt;&gt;instellingen!$G$2,ISBLANK($H19)),AND($G19=instellingen!$G$2,$H19&lt;&gt;"")),1,0)</f>
@@ -17105,7 +17118,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I20" s="45"/>
       <c r="J20" s="29" t="s">
@@ -17122,10 +17135,10 @@
         <v>2</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="R20" s="7">
         <f>IF(OR(AND($G20&lt;&gt;instellingen!$G$2,ISBLANK($H20)),AND($G20=instellingen!$G$2,$H20&lt;&gt;"")),1,0)</f>
@@ -18315,7 +18328,7 @@
       </c>
       <c r="F2" s="43">
         <f>SUM(AF6:AF35)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="49" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
@@ -18461,7 +18474,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2">
         <v>1007</v>
@@ -18471,7 +18484,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I6" s="45">
         <v>1</v>
@@ -18486,7 +18499,7 @@
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P6" s="32"/>
       <c r="R6" s="7">
@@ -18531,7 +18544,7 @@
       </c>
       <c r="AB6" s="7">
         <f>IF(AND(OR($O6=instellingen!$I$3,$O6=instellingen!$I$4),OR($M6=instellingen!$I$2,$M6=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="7">
         <f>IF(AND($O6=instellingen!$I$2,$M6=instellingen!$I$3),1,0)</f>
@@ -18547,7 +18560,7 @@
       </c>
       <c r="AF6" s="8">
         <f>SUM(R6:AE6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1" ht="72">
@@ -18565,7 +18578,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I7" s="45">
         <v>2</v>
@@ -18582,7 +18595,7 @@
       </c>
       <c r="N7" s="46"/>
       <c r="O7" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P7" s="32"/>
       <c r="R7" s="7">
@@ -18627,7 +18640,7 @@
       </c>
       <c r="AB7" s="7">
         <f>IF(AND(OR($O7=instellingen!$I$3,$O7=instellingen!$I$4),OR($M7=instellingen!$I$2,$M7=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="7">
         <f>IF(AND($O7=instellingen!$I$2,$M7=instellingen!$I$3),1,0)</f>
@@ -18643,7 +18656,7 @@
       </c>
       <c r="AF7" s="8">
         <f>SUM(R7:AE7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:32" customHeight="1" ht="72">
@@ -18661,7 +18674,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I8" s="45">
         <v>2</v>
@@ -18678,7 +18691,7 @@
       </c>
       <c r="N8" s="46"/>
       <c r="O8" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P8" s="32"/>
       <c r="R8" s="7">
@@ -18723,7 +18736,7 @@
       </c>
       <c r="AB8" s="7">
         <f>IF(AND(OR($O8=instellingen!$I$3,$O8=instellingen!$I$4),OR($M8=instellingen!$I$2,$M8=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="7">
         <f>IF(AND($O8=instellingen!$I$2,$M8=instellingen!$I$3),1,0)</f>
@@ -18739,7 +18752,7 @@
       </c>
       <c r="AF8" s="8">
         <f>SUM(R8:AE8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:32" customHeight="1" ht="72">
@@ -18758,7 +18771,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I9" s="45">
         <v>3</v>
@@ -18778,7 +18791,7 @@
         <v>11</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="R9" s="7">
         <f>IF(OR(AND($G9&lt;&gt;instellingen!$G$2,ISBLANK($H9)),AND($G9=instellingen!$G$2,$H9&lt;&gt;"")),1,0)</f>
@@ -18847,7 +18860,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2">
         <v>1011</v>
@@ -18857,7 +18870,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I10" s="45">
         <v>2</v>
@@ -18874,7 +18887,7 @@
       </c>
       <c r="N10" s="46"/>
       <c r="O10" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P10" s="32"/>
       <c r="R10" s="7">
@@ -18919,7 +18932,7 @@
       </c>
       <c r="AB10" s="7">
         <f>IF(AND(OR($O10=instellingen!$I$3,$O10=instellingen!$I$4),OR($M10=instellingen!$I$2,$M10=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="7">
         <f>IF(AND($O10=instellingen!$I$2,$M10=instellingen!$I$3),1,0)</f>
@@ -18935,7 +18948,7 @@
       </c>
       <c r="AF10" s="8">
         <f>SUM(R10:AE10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:32" customHeight="1" ht="72">
@@ -18954,7 +18967,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I11" s="45">
         <v>3</v>
@@ -18973,10 +18986,10 @@
         <v>1</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P11" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R11" s="7">
         <f>IF(OR(AND($G11&lt;&gt;instellingen!$G$2,ISBLANK($H11)),AND($G11=instellingen!$G$2,$H11&lt;&gt;"")),1,0)</f>
@@ -20605,7 +20618,7 @@
       </c>
       <c r="F2" s="43">
         <f>SUM(AF6:AF35)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G2" s="49" t="str">
         <f>IF(B14&gt;6,"verouderd PTA",CONCATENATE("Dit is het programma van de huidige ",B6,B14," (cohort ",B7," - ",B9,")"))</f>
@@ -20751,7 +20764,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D6" s="2">
         <v>180</v>
@@ -20761,7 +20774,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I6" s="45">
         <v>1</v>
@@ -20776,7 +20789,7 @@
       </c>
       <c r="N6" s="46"/>
       <c r="O6" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P6" s="32"/>
       <c r="R6" s="7">
@@ -20821,7 +20834,7 @@
       </c>
       <c r="AB6" s="7">
         <f>IF(AND(OR($O6=instellingen!$I$3,$O6=instellingen!$I$4),OR($M6=instellingen!$I$2,$M6=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="7">
         <f>IF(AND($O6=instellingen!$I$2,$M6=instellingen!$I$3),1,0)</f>
@@ -20837,7 +20850,7 @@
       </c>
       <c r="AF6" s="8">
         <f>SUM(R6:AE6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1" ht="72">
@@ -20855,7 +20868,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I7" s="45">
         <v>2</v>
@@ -20872,7 +20885,7 @@
       </c>
       <c r="N7" s="46"/>
       <c r="O7" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P7" s="32"/>
       <c r="R7" s="7">
@@ -20917,7 +20930,7 @@
       </c>
       <c r="AB7" s="7">
         <f>IF(AND(OR($O7=instellingen!$I$3,$O7=instellingen!$I$4),OR($M7=instellingen!$I$2,$M7=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="7">
         <f>IF(AND($O7=instellingen!$I$2,$M7=instellingen!$I$3),1,0)</f>
@@ -20933,7 +20946,7 @@
       </c>
       <c r="AF7" s="8">
         <f>SUM(R7:AE7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:32" customHeight="1" ht="72">
@@ -20951,7 +20964,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I8" s="45">
         <v>2</v>
@@ -20968,7 +20981,7 @@
       </c>
       <c r="N8" s="46"/>
       <c r="O8" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P8" s="32"/>
       <c r="R8" s="7">
@@ -21013,7 +21026,7 @@
       </c>
       <c r="AB8" s="7">
         <f>IF(AND(OR($O8=instellingen!$I$3,$O8=instellingen!$I$4),OR($M8=instellingen!$I$2,$M8=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="7">
         <f>IF(AND($O8=instellingen!$I$2,$M8=instellingen!$I$3),1,0)</f>
@@ -21029,7 +21042,7 @@
       </c>
       <c r="AF8" s="8">
         <f>SUM(R8:AE8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:32" customHeight="1" ht="72">
@@ -21048,7 +21061,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I9" s="45">
         <v>3</v>
@@ -21137,7 +21150,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44379.602349537</v>
+        <v>44385.633414352</v>
       </c>
       <c r="D10" s="2">
         <v>184</v>
@@ -21147,7 +21160,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I10" s="45">
         <v>2</v>
@@ -21164,7 +21177,7 @@
       </c>
       <c r="N10" s="46"/>
       <c r="O10" s="31" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="P10" s="32"/>
       <c r="R10" s="7">
@@ -21209,7 +21222,7 @@
       </c>
       <c r="AB10" s="7">
         <f>IF(AND(OR($O10=instellingen!$I$3,$O10=instellingen!$I$4),OR($M10=instellingen!$I$2,$M10=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="7">
         <f>IF(AND($O10=instellingen!$I$2,$M10=instellingen!$I$3),1,0)</f>
@@ -21225,7 +21238,7 @@
       </c>
       <c r="AF10" s="8">
         <f>SUM(R10:AE10)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:32" customHeight="1" ht="72">
@@ -21244,7 +21257,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I11" s="45">
         <v>3</v>
@@ -21263,10 +21276,10 @@
         <v>1</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P11" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R11" s="7">
         <f>IF(OR(AND($G11&lt;&gt;instellingen!$G$2,ISBLANK($H11)),AND($G11=instellingen!$G$2,$H11&lt;&gt;"")),1,0)</f>
@@ -21529,7 +21542,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="I18" s="45">
         <v>1</v>
@@ -21544,7 +21557,7 @@
       </c>
       <c r="N18" s="46"/>
       <c r="O18" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P18" s="32"/>
       <c r="R18" s="7">
@@ -21589,7 +21602,7 @@
       </c>
       <c r="AB18" s="7">
         <f>IF(AND(OR($O18=instellingen!$I$3,$O18=instellingen!$I$4),OR($M18=instellingen!$I$2,$M18=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="7">
         <f>IF(AND($O18=instellingen!$I$2,$M18=instellingen!$I$3),1,0)</f>
@@ -21605,7 +21618,7 @@
       </c>
       <c r="AF18" s="8">
         <f>SUM(R18:AE18)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:32" customHeight="1" ht="72">
@@ -21634,7 +21647,7 @@
       </c>
       <c r="N19" s="46"/>
       <c r="O19" s="31" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="P19" s="32"/>
       <c r="R19" s="7">
@@ -21679,7 +21692,7 @@
       </c>
       <c r="AB19" s="7">
         <f>IF(AND(OR($O19=instellingen!$I$3,$O19=instellingen!$I$4),OR($M19=instellingen!$I$2,$M19=instellingen!$I$4)),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="7">
         <f>IF(AND($O19=instellingen!$I$2,$M19=instellingen!$I$3),1,0)</f>
@@ -21695,7 +21708,7 @@
       </c>
       <c r="AF19" s="8">
         <f>SUM(R19:AE19)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1" ht="72">
@@ -21707,7 +21720,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I20" s="45">
         <v>3</v>
@@ -21726,10 +21739,10 @@
         <v>3</v>
       </c>
       <c r="O20" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="R20" s="7">
         <f>IF(OR(AND($G20&lt;&gt;instellingen!$G$2,ISBLANK($H20)),AND($G20=instellingen!$G$2,$H20&lt;&gt;"")),1,0)</f>
@@ -21801,7 +21814,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="I21" s="45">
         <v>3</v>
@@ -21820,10 +21833,10 @@
         <v>1</v>
       </c>
       <c r="O21" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P21" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="R21" s="7">
         <f>IF(OR(AND($G21&lt;&gt;instellingen!$G$2,ISBLANK($H21)),AND($G21=instellingen!$G$2,$H21&lt;&gt;"")),1,0)</f>
@@ -21895,7 +21908,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="I22" s="45">
         <v>3</v>
@@ -21909,13 +21922,13 @@
         <v>8</v>
       </c>
       <c r="N22" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22" s="31" t="s">
         <v>11</v>
       </c>
       <c r="P22" s="32" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="R22" s="7">
         <f>IF(OR(AND($G22&lt;&gt;instellingen!$G$2,ISBLANK($H22)),AND($G22=instellingen!$G$2,$H22&lt;&gt;"")),1,0)</f>
@@ -21987,7 +22000,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I23" s="45">
         <v>3</v>
@@ -22006,10 +22019,10 @@
         <v>2</v>
       </c>
       <c r="O23" s="31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P23" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R23" s="7">
         <f>IF(OR(AND($G23&lt;&gt;instellingen!$G$2,ISBLANK($H23)),AND($G23=instellingen!$G$2,$H23&lt;&gt;"")),1,0)</f>

</xml_diff>